<commit_message>
crud size and mausac v_1
</commit_message>
<xml_diff>
--- a/loai-excel.xlsx
+++ b/loai-excel.xlsx
@@ -1,41 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20363"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DuAnToTNghiep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATN\DuAnTotNghiep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F94D26-312E-4052-B0F9-F93E49935FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F596269-1CDA-468F-BABB-A739F1D3A84A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6990" yWindow="3180" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{FCB1BF08-13B3-42C4-A4EC-5E0B0AC07D29}"/>
+    <workbookView xWindow="6990" yWindow="3180" windowWidth="17280" windowHeight="8880" activeTab="4" xr2:uid="{FCB1BF08-13B3-42C4-A4EC-5E0B0AC07D29}"/>
   </bookViews>
   <sheets>
     <sheet name="loai" sheetId="1" r:id="rId1"/>
     <sheet name="thuong hieu" sheetId="2" r:id="rId2"/>
     <sheet name="san pham" sheetId="3" r:id="rId3"/>
+    <sheet name="size" sheetId="4" r:id="rId4"/>
+    <sheet name="mausac" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>tên</t>
   </si>
@@ -86,6 +80,15 @@
   </si>
   <si>
     <t>có thể tháo rời</t>
+  </si>
+  <si>
+    <t>trangthai</t>
+  </si>
+  <si>
+    <t>XXL</t>
+  </si>
+  <si>
+    <t>Kem</t>
   </si>
 </sst>
 </file>
@@ -96,7 +99,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -444,9 +447,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,7 +457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -462,7 +465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -470,7 +473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -491,9 +494,9 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -501,7 +504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -509,7 +512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -526,20 +529,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B9D7AB2-2C84-4048-87E4-848F92812618}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.375" customWidth="1"/>
-    <col min="3" max="3" width="25.875" customWidth="1"/>
-    <col min="4" max="4" width="23.25" customWidth="1"/>
-    <col min="5" max="5" width="25.75" customWidth="1"/>
-    <col min="6" max="6" width="14.375" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" customWidth="1"/>
+    <col min="3" max="3" width="25.90625" customWidth="1"/>
+    <col min="4" max="4" width="23.26953125" customWidth="1"/>
+    <col min="5" max="5" width="25.7265625" customWidth="1"/>
+    <col min="6" max="6" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -562,7 +565,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -583,6 +586,68 @@
       </c>
       <c r="G2">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A92A7BCA-71B4-45AE-A7A8-B7A3A8FD067A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2080EE-35BC-4CF7-9CDA-6BBFA323AF1E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sửa mysql_script và thêm excel san pham chi tiet
</commit_message>
<xml_diff>
--- a/loai-excel.xlsx
+++ b/loai-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DuAnToTNghiep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFD2389-29C1-4E77-BB91-011EC75D0E60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13BA58F-DA23-4352-A4E2-A0A88B7E0862}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{FCB1BF08-13B3-42C4-A4EC-5E0B0AC07D29}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{FCB1BF08-13B3-42C4-A4EC-5E0B0AC07D29}"/>
   </bookViews>
   <sheets>
     <sheet name="loai" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>tên</t>
   </si>
@@ -110,17 +110,69 @@
     <t>số lượng</t>
   </si>
   <si>
-    <t>ảnh</t>
+    <t>id mau sac</t>
+  </si>
+  <si>
+    <t>id size</t>
+  </si>
+  <si>
+    <t>số lượng size</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>1,2,3,4</t>
+  </si>
+  <si>
+    <t>1,2,4</t>
+  </si>
+  <si>
+    <t>ảnh màu sắc</t>
+  </si>
+  <si>
+    <t>https://royalhelmet.com.vn/ckfinder/userfiles/images/products/Zt7RKI_MG_3349.jpg ,https://royalhelmet.com.vn/ckfinder/userfiles/images/products/P0jXDB_MG_3354.jpg,https://royalhelmet.com.vn/ckfinder/userfiles/images/products/K6uk81_MG_3354-muc.jpg</t>
+  </si>
+  <si>
+    <t>mô tả màu sắc</t>
+  </si>
+  <si>
+    <t>1,2,4,4</t>
+  </si>
+  <si>
+    <t>ảnh chính</t>
+  </si>
+  <si>
+    <t>https://royalhelmet.com.vn/ckfinder/userfiles/images/products/klIZba_MG_3349.jpg, https://royalhelmet.com.vn/ckfinder/userfiles/images/products/TLXYEi_MG_3350.jpg,https://royalhelmet.com.vn/ckfinder/userfiles/images/products/NOYMt4_MG_3352.jpg</t>
+  </si>
+  <si>
+    <t>https://royalhelmet.com.vn/ckfinder/userfiles/images/products/b4hEP5SwGTU0royal-m139-v7.jpg,https://royalhelmet.com.vn/ckfinder/userfiles/images/products/3IqhWcroyal-m139-v7-1.jpg,https://royalhelmet.com.vn/ckfinder/userfiles/images/products/hD1uIXroyal-m139-v7-2.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
@@ -144,13 +196,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -617,19 +672,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D237B75-BB31-4251-A09F-AD1A4753482D}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.25" customWidth="1"/>
     <col min="4" max="4" width="16.25" customWidth="1"/>
+    <col min="8" max="8" width="11.5" customWidth="1"/>
+    <col min="10" max="11" width="14.25" customWidth="1"/>
+    <col min="12" max="12" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -654,8 +712,107 @@
       <c r="H1" t="s">
         <v>24</v>
       </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>20000</v>
+      </c>
+      <c r="F2">
+        <v>20000</v>
+      </c>
+      <c r="G2">
+        <v>54</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>121</v>
+      </c>
+      <c r="F3">
+        <v>213</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{2102CD33-D624-44F2-84E3-3701D98629CD}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{F018848B-ED07-4873-A516-AC4B3C9BD743}"/>
+    <hyperlink ref="M2" r:id="rId3" display="https://royalhelmet.com.vn/ckfinder/userfiles/images/products/klIZba_MG_3349.jpg" xr:uid="{117169F8-945C-4E9E-B609-AD42B10E3DA5}"/>
+    <hyperlink ref="M3" r:id="rId4" display="https://royalhelmet.com.vn/ckfinder/userfiles/images/products/b4hEP5SwGTU0royal-m139-v7.jpg,https://royalhelmet.com.vn/ckfinder/userfiles/images/products/3IqhWcroyal-m139-v7-1.jpg,https://royalhelmet.com.vn/ckfinder/userfiles/images/products/hD1uIXroyal-m139-v7-2.jpg" xr:uid="{4E885543-461C-4B9D-8900-D02B5D55EA6C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sửa lại thêm bằng excel(tồn tại thì update ko thì thêm mới)
</commit_message>
<xml_diff>
--- a/loai-excel.xlsx
+++ b/loai-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DuAnToTNghiep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13BA58F-DA23-4352-A4E2-A0A88B7E0862}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76A5E91-65A6-496B-82E2-3D34F0FD34A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{FCB1BF08-13B3-42C4-A4EC-5E0B0AC07D29}"/>
+    <workbookView xWindow="3600" yWindow="2880" windowWidth="20445" windowHeight="10485" xr2:uid="{FCB1BF08-13B3-42C4-A4EC-5E0B0AC07D29}"/>
   </bookViews>
   <sheets>
     <sheet name="loai" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>ao</t>
   </si>
   <si>
-    <t>dep</t>
-  </si>
-  <si>
     <t>ten</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>https://royalhelmet.com.vn/ckfinder/userfiles/images/products/b4hEP5SwGTU0royal-m139-v7.jpg,https://royalhelmet.com.vn/ckfinder/userfiles/images/products/3IqhWcroyal-m139-v7-1.jpg,https://royalhelmet.com.vn/ckfinder/userfiles/images/products/hD1uIXroyal-m139-v7-2.jpg</t>
+  </si>
+  <si>
+    <t>Xe đạp</t>
   </si>
 </sst>
 </file>
@@ -200,9 +200,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -520,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D77F84-41E5-4310-9187-F262CB499DDF}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -551,8 +554,8 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
+      <c r="A4" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -575,7 +578,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -583,7 +586,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -591,7 +594,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -621,42 +624,42 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -674,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D237B75-BB31-4251-A09F-AD1A4753482D}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -689,43 +692,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" t="s">
-        <v>26</v>
-      </c>
       <c r="K1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -751,24 +754,24 @@
         <v>54</v>
       </c>
       <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
         <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
       </c>
       <c r="J2">
         <v>3</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -789,19 +792,19 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J3">
         <v>3</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
them so_luong vao vouvcher và sua lai them excel san pham chi tiet
</commit_message>
<xml_diff>
--- a/loai-excel.xlsx
+++ b/loai-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DuAnToTNghiep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287466C4-2F1F-4A38-9467-2AB0BA4A274C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4FED9E-6212-47DE-AD87-B3EFB1F7766A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{FCB1BF08-13B3-42C4-A4EC-5E0B0AC07D29}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>tên</t>
   </si>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>Xe đạp</t>
-  </si>
-  <si>
-    <t>sssssssssssss</t>
   </si>
 </sst>
 </file>
@@ -312,6 +309,206 @@
         <a:xfrm>
           <a:off x="15097125" y="1685925"/>
           <a:ext cx="1038224" cy="1038224"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>981074</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1057274</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7915206-2C95-47D0-B3A9-4AFB1EB024C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12277725" y="466725"/>
+          <a:ext cx="771524" cy="771524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1437073</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>867352</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA54D1B9-F95F-45F1-8E4C-CAE63548A422}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12420600" y="1895475"/>
+          <a:ext cx="1084648" cy="610177"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1396998</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>419099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2446866</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1009650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFDEFFB2-010A-44D5-8E63-AFEC653DFFE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13465173" y="600074"/>
+          <a:ext cx="1049868" cy="590551"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2586566</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>314324</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>3924300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1066799</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60DFCDBD-DF1E-4F74-8340-1273C0F6ED20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14654741" y="495299"/>
+          <a:ext cx="1337734" cy="752475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -777,7 +974,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -787,7 +984,7 @@
     <col min="8" max="8" width="11.5" customWidth="1"/>
     <col min="10" max="10" width="14.25" customWidth="1"/>
     <col min="11" max="11" width="48.125" customWidth="1"/>
-    <col min="12" max="12" width="24.625" customWidth="1"/>
+    <col min="12" max="12" width="56" customWidth="1"/>
     <col min="13" max="13" width="36.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -863,9 +1060,7 @@
       <c r="J2">
         <v>3</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
sua them excel image vao chi tiet san pham
</commit_message>
<xml_diff>
--- a/loai-excel.xlsx
+++ b/loai-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DuAnToTNghiep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4FED9E-6212-47DE-AD87-B3EFB1F7766A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5FBC6F-5DBD-4038-A4F7-2B2738C87DC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{FCB1BF08-13B3-42C4-A4EC-5E0B0AC07D29}"/>
   </bookViews>
@@ -122,22 +122,22 @@
     <t>1,2,3,4</t>
   </si>
   <si>
-    <t>1,2,4</t>
-  </si>
-  <si>
     <t>ảnh màu sắc</t>
   </si>
   <si>
     <t>mô tả màu sắc</t>
   </si>
   <si>
-    <t>1,2,4,4</t>
-  </si>
-  <si>
     <t>ảnh chính</t>
   </si>
   <si>
     <t>Xe đạp</t>
+  </si>
+  <si>
+    <t>D:\anh\digital-art-artwork-illustration-digital-painting-pink-hd-wallpaper-cc923972d4ec819cccf9880f8b916d69.jpg</t>
+  </si>
+  <si>
+    <t>D:\anh\318500342_195400319734317_2076385213486251926_n.jpg,D:\anh\28.png,D:\anh\18.jpg,D:\anh\318500342_195400319734317_2076385213486251926_n.jpg</t>
   </si>
 </sst>
 </file>
@@ -213,311 +213,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>352424</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>172640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>2362200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1303138</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0465C59A-035E-4DB7-9C93-60B004E0FEBA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14297024" y="353615"/>
-          <a:ext cx="2009776" cy="1130498"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>1152525</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>2190749</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1085849</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A15D7913-EF35-43A2-9833-9CBAC95EBD9A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15097125" y="1685925"/>
-          <a:ext cx="1038224" cy="1038224"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>285750</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>981074</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1057274</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7915206-2C95-47D0-B3A9-4AFB1EB024C8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12277725" y="466725"/>
-          <a:ext cx="771524" cy="771524"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>257175</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1437073</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>867352</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA54D1B9-F95F-45F1-8E4C-CAE63548A422}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="12420600" y="1895475"/>
-          <a:ext cx="1084648" cy="610177"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1396998</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>419099</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>2446866</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1009650</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFDEFFB2-010A-44D5-8E63-AFEC653DFFE4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13465173" y="600074"/>
-          <a:ext cx="1049868" cy="590551"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>2586566</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>314324</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>3924300</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1066799</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60DFCDBD-DF1E-4F74-8340-1273C0F6ED20}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14654741" y="495299"/>
-          <a:ext cx="1337734" cy="752475"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -851,7 +546,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -971,10 +666,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D237B75-BB31-4251-A09F-AD1A4753482D}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1020,13 +715,13 @@
         <v>25</v>
       </c>
       <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
         <v>30</v>
-      </c>
-      <c r="L1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1060,47 +755,16 @@
       <c r="J2">
         <v>3</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>25</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>121</v>
-      </c>
-      <c r="F3">
-        <v>213</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3">
-        <v>3</v>
-      </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="L2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
hoàn thành add sản phẩm
</commit_message>
<xml_diff>
--- a/loai-excel.xlsx
+++ b/loai-excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DuAnToTNghiep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\do-an\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5FBC6F-5DBD-4038-A4F7-2B2738C87DC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0A38BB-84F2-4E30-9FF1-BFFE353A1E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{FCB1BF08-13B3-42C4-A4EC-5E0B0AC07D29}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{FCB1BF08-13B3-42C4-A4EC-5E0B0AC07D29}"/>
   </bookViews>
   <sheets>
     <sheet name="loai" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>tên</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>D:\anh\318500342_195400319734317_2076385213486251926_n.jpg,D:\anh\28.png,D:\anh\18.jpg,D:\anh\318500342_195400319734317_2076385213486251926_n.jpg</t>
+  </si>
+  <si>
+    <t>ROYAL M20D</t>
+  </si>
+  <si>
+    <t>xốp EPS</t>
   </si>
 </sst>
 </file>
@@ -148,14 +154,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -164,7 +170,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -518,9 +524,9 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -528,7 +534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -536,7 +542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -544,7 +550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
@@ -565,9 +571,9 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -575,7 +581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -583,7 +589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -604,16 +610,16 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.375" customWidth="1"/>
-    <col min="3" max="3" width="25.875" customWidth="1"/>
-    <col min="4" max="4" width="23.25" customWidth="1"/>
-    <col min="5" max="5" width="25.75" customWidth="1"/>
-    <col min="6" max="6" width="14.375" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -636,7 +642,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -668,22 +674,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D237B75-BB31-4251-A09F-AD1A4753482D}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.25" customWidth="1"/>
-    <col min="4" max="4" width="16.25" customWidth="1"/>
-    <col min="8" max="8" width="11.5" customWidth="1"/>
-    <col min="10" max="10" width="14.25" customWidth="1"/>
-    <col min="11" max="11" width="48.125" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
+    <col min="11" max="11" width="48.140625" customWidth="1"/>
     <col min="12" max="12" width="56" customWidth="1"/>
-    <col min="13" max="13" width="36.625" customWidth="1"/>
+    <col min="13" max="13" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -724,18 +730,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
+    <row r="2" spans="1:13" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
+      <c r="C2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="2">
+        <v>850</v>
       </c>
       <c r="E2">
         <v>20000</v>

</xml_diff>

<commit_message>
cập nhập excel thêm sản phẩm
</commit_message>
<xml_diff>
--- a/loai-excel.xlsx
+++ b/loai-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\do-an\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0A38BB-84F2-4E30-9FF1-BFFE353A1E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5238A56E-0D4F-42C6-A500-BC2D2A09A6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{FCB1BF08-13B3-42C4-A4EC-5E0B0AC07D29}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="loai" sheetId="1" r:id="rId1"/>
     <sheet name="thuong hieu" sheetId="2" r:id="rId2"/>
     <sheet name="san pham" sheetId="3" r:id="rId3"/>
-    <sheet name="chi tiet sp" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>tên</t>
   </si>
@@ -86,18 +86,9 @@
     <t>có thể tháo rời</t>
   </si>
   <si>
-    <t>id sản phẩm</t>
-  </si>
-  <si>
     <t>trạng thái</t>
   </si>
   <si>
-    <t>id vật liệu</t>
-  </si>
-  <si>
-    <t>id trọng lượng</t>
-  </si>
-  <si>
     <t>giá bán</t>
   </si>
   <si>
@@ -140,27 +131,59 @@
     <t>D:\anh\318500342_195400319734317_2076385213486251926_n.jpg,D:\anh\28.png,D:\anh\18.jpg,D:\anh\318500342_195400319734317_2076385213486251926_n.jpg</t>
   </si>
   <si>
-    <t>ROYAL M20D</t>
-  </si>
-  <si>
-    <t>xốp EPS</t>
+    <t>nhựa ABS nguyên sinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> trọng lượng</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vật liệu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sản phẩm</t>
+  </si>
+  <si>
+    <t>màu đen ánh đỏ</t>
+  </si>
+  <si>
+    <t>quai 1</t>
+  </si>
+  <si>
+    <t>quai đeo</t>
+  </si>
+  <si>
+    <t>đệm lót</t>
+  </si>
+  <si>
+    <t>đệm 1</t>
+  </si>
+  <si>
+    <t>mô tả sản phẩm</t>
+  </si>
+  <si>
+    <t>sản phẩm mới ra mắt</t>
+  </si>
+  <si>
+    <t>loại sản phẩm</t>
+  </si>
+  <si>
+    <t>Thương hiệu</t>
+  </si>
+  <si>
+    <t>Amoro</t>
+  </si>
+  <si>
+    <t>hoang</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="163"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
@@ -195,13 +218,21 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -551,8 +582,8 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>31</v>
+      <c r="A4" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -671,106 +702,135 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D237B75-BB31-4251-A09F-AD1A4753482D}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95998B40-D9B1-4850-A3A1-BC05E4CB85A0}">
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" customWidth="1"/>
-    <col min="11" max="11" width="48.140625" customWidth="1"/>
-    <col min="12" max="12" width="56" customWidth="1"/>
-    <col min="13" max="13" width="36.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="11" max="11" width="55.140625" customWidth="1"/>
+    <col min="12" max="12" width="26" customWidth="1"/>
+    <col min="16" max="16" width="25.85546875" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" t="s">
-        <v>28</v>
-      </c>
       <c r="M1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2">
+        <v>45</v>
+      </c>
+      <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2">
         <v>850</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>20000</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>20000</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>54</v>
       </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2">
+      <c r="H2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="3">
         <v>3</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>32</v>
+      <c r="K2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sửa đang nhập gg
</commit_message>
<xml_diff>
--- a/loai-excel.xlsx
+++ b/loai-excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\do-an\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\dangNhapGG\DuAnTotNghiep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5238A56E-0D4F-42C6-A500-BC2D2A09A6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1F648F-11EB-44BB-8876-85F7BD702764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{FCB1BF08-13B3-42C4-A4EC-5E0B0AC07D29}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{FCB1BF08-13B3-42C4-A4EC-5E0B0AC07D29}"/>
   </bookViews>
   <sheets>
     <sheet name="loai" sheetId="1" r:id="rId1"/>
@@ -125,12 +125,6 @@
     <t>Xe đạp</t>
   </si>
   <si>
-    <t>D:\anh\digital-art-artwork-illustration-digital-painting-pink-hd-wallpaper-cc923972d4ec819cccf9880f8b916d69.jpg</t>
-  </si>
-  <si>
-    <t>D:\anh\318500342_195400319734317_2076385213486251926_n.jpg,D:\anh\28.png,D:\anh\18.jpg,D:\anh\318500342_195400319734317_2076385213486251926_n.jpg</t>
-  </si>
-  <si>
     <t>nhựa ABS nguyên sinh</t>
   </si>
   <si>
@@ -174,6 +168,12 @@
   </si>
   <si>
     <t>hoang</t>
+  </si>
+  <si>
+    <t>D:\imgDATN\2.png</t>
+  </si>
+  <si>
+    <t>D:\imgDATN\3.png</t>
   </si>
 </sst>
 </file>
@@ -555,9 +555,9 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -565,7 +565,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -573,7 +573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -581,7 +581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -602,9 +602,9 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -612,7 +612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -620,7 +620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -641,16 +641,16 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -673,7 +673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -705,31 +705,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95998B40-D9B1-4850-A3A1-BC05E4CB85A0}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
-    <col min="11" max="11" width="55.140625" customWidth="1"/>
+    <col min="10" max="10" width="20.109375" customWidth="1"/>
+    <col min="11" max="11" width="55.109375" customWidth="1"/>
     <col min="12" max="12" width="26" customWidth="1"/>
-    <col min="16" max="16" width="25.85546875" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" customWidth="1"/>
+    <col min="16" max="16" width="25.88671875" customWidth="1"/>
+    <col min="17" max="17" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
         <v>17</v>
@@ -759,30 +759,30 @@
         <v>27</v>
       </c>
       <c r="N1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="O1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" t="s">
         <v>38</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" t="s">
-        <v>42</v>
-      </c>
       <c r="R1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2">
         <v>850</v>
@@ -806,28 +806,28 @@
         <v>3</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="O2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>